<commit_message>
Add document clasifier script
</commit_message>
<xml_diff>
--- a/resultados/Naive Bayes/predicciones-brenoulli.xlsx
+++ b/resultados/Naive Bayes/predicciones-brenoulli.xlsx
@@ -460,13 +460,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="3">
@@ -488,13 +488,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="5">
@@ -533,10 +533,10 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.09</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +558,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.66</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -575,10 +575,10 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.72</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0.28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +586,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="12">
@@ -617,10 +617,10 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -628,10 +628,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -642,13 +642,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -659,10 +659,10 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -670,13 +670,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.79</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0.09</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -684,13 +684,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -715,10 +715,10 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -743,10 +743,10 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -754,13 +754,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>0.99</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="24">
@@ -768,10 +768,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -782,13 +782,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>0.99</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -838,13 +838,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -852,13 +852,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.32</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>0.13</v>
+        <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>0.55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -869,10 +869,10 @@
         <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -883,10 +883,10 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -894,13 +894,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -911,10 +911,10 @@
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -922,13 +922,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -939,10 +939,10 @@
         <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -950,10 +950,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
@@ -981,10 +981,10 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="D39" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="40">
@@ -992,13 +992,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" t="n">
-        <v>0.99</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1006,10 +1006,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
@@ -1020,13 +1020,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="43">
@@ -1037,10 +1037,10 @@
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1048,10 +1048,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
@@ -1062,13 +1062,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -1076,13 +1076,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1090,10 +1090,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
@@ -1104,10 +1104,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
@@ -1118,10 +1118,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" t="n">
         <v>0</v>
@@ -1132,10 +1132,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" t="n">
         <v>0</v>
@@ -1163,10 +1163,10 @@
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -1174,13 +1174,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -1188,13 +1188,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="C54" t="n">
-        <v>1</v>
+        <v>0.79</v>
       </c>
       <c r="D54" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="55">
@@ -1230,10 +1230,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
         <v>0</v>
@@ -1244,13 +1244,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58" t="n">
         <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -1258,13 +1258,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -1275,10 +1275,10 @@
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="61">
@@ -1286,10 +1286,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D61" t="n">
         <v>0</v>
@@ -1303,10 +1303,10 @@
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>0.99</v>
       </c>
       <c r="D62" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="63">
@@ -1328,13 +1328,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64" t="n">
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -1359,10 +1359,10 @@
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -1373,10 +1373,10 @@
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="68">
@@ -1384,13 +1384,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="C68" t="n">
-        <v>1</v>
+        <v>0.66</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="69">
@@ -1398,10 +1398,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69" t="n">
         <v>0</v>
@@ -1415,10 +1415,10 @@
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -1426,13 +1426,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>0.89</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -1440,13 +1440,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="C72" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1457,10 +1457,10 @@
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>0.99</v>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="74">
@@ -1496,10 +1496,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D76" t="n">
         <v>0</v>
@@ -1538,13 +1538,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C79" t="n">
-        <v>0.98</v>
+        <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -1555,10 +1555,10 @@
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -1569,10 +1569,10 @@
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>0.72</v>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="82">
@@ -1597,10 +1597,10 @@
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -1611,10 +1611,10 @@
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="D84" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -1622,13 +1622,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C85" t="n">
-        <v>0.99</v>
+        <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -1636,13 +1636,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" t="n">
         <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -1650,13 +1650,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>1</v>
+        <v>0.32</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="88">
@@ -1664,10 +1664,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D88" t="n">
         <v>0</v>
@@ -1678,10 +1678,10 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89" t="n">
         <v>0</v>
@@ -1692,13 +1692,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.74</v>
+        <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>0.13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -1706,13 +1706,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C91" t="n">
         <v>0</v>
       </c>
       <c r="D91" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>